<commit_message>
refactor: Deleted all unused classes
</commit_message>
<xml_diff>
--- a/src/Resources/SnakeeLeaderboard.xlsx
+++ b/src/Resources/SnakeeLeaderboard.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -447,7 +447,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD05B22-988A-4146-BED8-42077AB0D08E}">
-  <dimension ref="A1:B88"/>
+  <dimension ref="A1:B89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -1155,6 +1155,14 @@
       </c>
       <c r="B88" t="n" s="0">
         <v>4168.0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B89" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>